<commit_message>
registeUser() with negavite data scenarios
</commit_message>
<xml_diff>
--- a/java/Hybrid/util/InputData.xlsx
+++ b/java/Hybrid/util/InputData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="62">
   <si>
     <t xml:space="preserve">Email ID</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t xml:space="preserve">all invalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valid data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test(random num)@mailinator.com</t>
   </si>
   <si>
     <t xml:space="preserve">LoginButton disability</t>
@@ -337,19 +346,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -984,10 +995,20 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B69" s="4"/>
+      <c r="A69" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1042,18 +1063,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1061,107 +1083,107 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1169,29 +1191,29 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1227,24 +1249,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>